<commit_message>
Updates to tutorial files as per reviewer requests
</commit_message>
<xml_diff>
--- a/analysis/nutritionToolbox/inputData/demoCreateDiet.xlsx
+++ b/analysis/nutritionToolbox/inputData/demoCreateDiet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nuigalwayie.sharepoint.com/sites/Group_MSP/Shared Documents/Projects/ViennaDiet/submissionNT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{96F62136-E14B-43CB-8CDE-D44216E3AE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EF46A38-AA8D-4844-8F31-578F52FA08F2}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{96F62136-E14B-43CB-8CDE-D44216E3AE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C06C005-77CB-4240-A3BA-77BBADAEAF34}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{81D3A005-C3AC-41DA-9482-692B44B023C1}"/>
   </bookViews>
@@ -604,6 +604,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1003,27 +1006,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="115d27ae-6a50-4eec-a8c0-aa0138fe553c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c759ece7-115b-4d09-a992-0736880850b1" xsi:nil="true"/>
-    <Keyword xmlns="115d27ae-6a50-4eec-a8c0-aa0138fe553c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D951DA713A5BE4DB914422C145C765D" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="187661b5ba509de40c852abd4410bd3b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="115d27ae-6a50-4eec-a8c0-aa0138fe553c" xmlns:ns3="c759ece7-115b-4d09-a992-0736880850b1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f6e787b82b781108b21eaa2fc08711e2" ns2:_="" ns3:_="">
     <xsd:import namespace="115d27ae-6a50-4eec-a8c0-aa0138fe553c"/>
@@ -1286,26 +1268,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39FD0494-F7D2-4593-A48E-B33F5122E1EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="115d27ae-6a50-4eec-a8c0-aa0138fe553c"/>
-    <ds:schemaRef ds:uri="c759ece7-115b-4d09-a992-0736880850b1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D9E073D-236B-4338-8F7A-580E65EC7066}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="115d27ae-6a50-4eec-a8c0-aa0138fe553c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c759ece7-115b-4d09-a992-0736880850b1" xsi:nil="true"/>
+    <Keyword xmlns="115d27ae-6a50-4eec-a8c0-aa0138fe553c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CE3E31F-C459-483F-A174-538CC6222D5F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1322,4 +1306,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D9E073D-236B-4338-8F7A-580E65EC7066}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39FD0494-F7D2-4593-A48E-B33F5122E1EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="115d27ae-6a50-4eec-a8c0-aa0138fe553c"/>
+    <ds:schemaRef ds:uri="c759ece7-115b-4d09-a992-0736880850b1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>